<commit_message>
load data netsuite to datalake, datawarehouse
</commit_message>
<xml_diff>
--- a/db/results/tara/dmcl_tara.xlsx
+++ b/db/results/tara/dmcl_tara.xlsx
@@ -891,12 +891,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>290.000đ</t>
+          <t>270.000đ</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>290.000đ</t>
+          <t>270.000đ</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -991,12 +991,12 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>6.790.000đ</t>
+          <t>6.290.000đ</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>6.790.000đ</t>
+          <t>6.290.000đ</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1023,12 +1023,12 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>10.990.000đ</t>
+          <t>10.490.000đ</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>10.990.000đ</t>
+          <t>10.490.000đ</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1131,12 +1131,12 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>419.000đ</t>
+          <t>390.000đ</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>419.000đ</t>
+          <t>390.000đ</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">

</xml_diff>